<commit_message>
Integrate sensor and Bluetooth arduino code
* Update excel sheet with correlation plot

* Clean sensor arduino code
</commit_message>
<xml_diff>
--- a/Matlab/sensor-data.xlsx
+++ b/Matlab/sensor-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sfuca0-my.sharepoint.com/personal/kammar_sfuca0_onmicrosoft_com/Documents/Desktop/Spring 2021/ENSC 405W/Project/Workspace/company-8-project/Matlab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="426" documentId="8_{00813D6E-801C-4654-9E05-4789C4C7A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{21EDA69F-515F-4765-90C0-3D4F10F4AC62}"/>
+  <xr:revisionPtr revIDLastSave="438" documentId="8_{00813D6E-801C-4654-9E05-4789C4C7A1C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41931FC9-2468-486D-ACEA-C1AB24A236CF}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="10190" firstSheet="4" activeTab="8" xr2:uid="{8DB2FC07-4C4E-4436-8775-2880AF42DB29}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19190" windowHeight="10190" firstSheet="5" activeTab="8" xr2:uid="{8DB2FC07-4C4E-4436-8775-2880AF42DB29}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="28">
   <si>
     <t>NormSCG</t>
   </si>
@@ -128,9 +128,6 @@
   </si>
   <si>
     <t>Average Difference</t>
-  </si>
-  <si>
-    <t>Correaltion</t>
   </si>
   <si>
     <t>Correlation</t>
@@ -3434,6 +3431,749 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Blood Pressure Estimation Correlation</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Aggregate mPTP'!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Aggregate mPTP'!$B$2:$B$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>54</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-59F1-42A5-8B38-44F8740568C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Aggregate mPTP'!$A$2:$A$28</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="27"/>
+                <c:pt idx="0">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>66</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>59</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Aggregate mPTP'!$I$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>0.87122883206193491</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-59F1-42A5-8B38-44F8740568C3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="675262096"/>
+        <c:axId val="675255864"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="675262096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="50"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Estimated Blood Pressure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.48228346456692911"/>
+              <c:y val="0.87868037328667248"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="675255864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="675255864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="45"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Real Blood Pressure</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="675262096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:userShapes r:id="rId3"/>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="50" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
@@ -4375,6 +5115,46 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -6487,6 +7267,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="249">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7171,10 +8467,92 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>141193</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>115794</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>82922</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41ACBD48-6ACA-4CBD-8B2A-DF9739891D1A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.14624</cdr:x>
+      <cdr:y>0.18546</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.31944</cdr:x>
+      <cdr:y>0.29711</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F121C270-764D-4590-BC97-897CB581484C}"/>
+            </a:ext>
+          </a:extLst>
+        </cdr:cNvPr>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="668618" y="508748"/>
+          <a:ext cx="791882" cy="306294"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="square" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-CA" sz="1100"/>
+            <a:t>R = 0.87</a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -19876,7 +21254,7 @@
     </row>
     <row r="23" spans="9:10" x14ac:dyDescent="0.35">
       <c r="I23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J23">
         <f>CORREL(B2:B10, C2:C10)</f>
@@ -40249,8 +41627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A171961-2335-46B0-AEFC-F66A210A2D1B}">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+    <sheetView tabSelected="1" topLeftCell="B16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>